<commit_message>
HighLight and Properties file
Completed the code for Highlighting an element and reading data from the properties file.
</commit_message>
<xml_diff>
--- a/Resources/TestData.xlsx
+++ b/Resources/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\All_In_One\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4869FB69-CD81-4D57-9BF5-66A9B8ADB969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377F48F3-1291-439A-9F74-04488C8525AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alphaSheet" sheetId="1" r:id="rId1"/>
     <sheet name="betaSheet" sheetId="2" r:id="rId2"/>
+    <sheet name="realTime" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
   <si>
     <t>attribute1</t>
   </si>
@@ -229,9 +230,6 @@
     <t>1235</t>
   </si>
   <si>
-    <t>1236</t>
-  </si>
-  <si>
     <t>1237</t>
   </si>
   <si>
@@ -245,6 +243,27 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>HighLightElement</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>passWord</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>12456</t>
+  </si>
+  <si>
+    <t>786</t>
   </si>
 </sst>
 </file>
@@ -621,25 +640,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="8"/>
-    <col min="10" max="10" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="8"/>
+    <col min="10" max="10" width="9.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -665,7 +684,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="5" t="s">
         <v>54</v>
@@ -686,7 +705,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
@@ -706,7 +725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
         <v>18</v>
@@ -721,7 +740,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
@@ -747,7 +766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>65</v>
@@ -756,19 +775,19 @@
         <v>66</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
@@ -806,7 +825,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>64</v>
@@ -839,9 +858,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>48</v>
@@ -856,22 +875,22 @@
         <v>51</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -886,22 +905,22 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -927,7 +946,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -948,7 +967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>43</v>
       </c>
@@ -968,7 +987,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -983,7 +1002,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -1009,7 +1028,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -1030,7 +1049,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -1068,7 +1087,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>21</v>
@@ -1104,4 +1123,49 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0703D59-0802-4774-9111-52139DE76A14}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>